<commit_message>
Fix mibi syntax and regen
</commit_message>
<xml_diff>
--- a/docs/mibi/mibi-metadata.xlsx
+++ b/docs/mibi/mibi-metadata.xlsx
@@ -14,9 +14,9 @@
     <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
     <sheet name="resolution_x_unit list" sheetId="6" r:id="rId6"/>
     <sheet name="resolution_y_unit list" sheetId="7" r:id="rId7"/>
-    <sheet name="area_normalize...dose_unit list" sheetId="8" r:id="rId8"/>
-    <sheet name="max_x_width_unit list" sheetId="9" r:id="rId9"/>
-    <sheet name="max_y_height_unit list" sheetId="10" r:id="rId10"/>
+    <sheet name="max_x_width_unit list" sheetId="8" r:id="rId8"/>
+    <sheet name="max_y_height_unit list" sheetId="9" r:id="rId9"/>
+    <sheet name="area_normalize...dose_unit list" sheetId="10" r:id="rId10"/>
     <sheet name="pixel_dwell_time_unit list" sheetId="11" r:id="rId11"/>
     <sheet name="pixel_size_x_unit list" sheetId="12" r:id="rId12"/>
     <sheet name="pixel_size_y_unit list" sheetId="13" r:id="rId13"/>
@@ -306,11 +306,102 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Image width value of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of image width of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Image height value of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units of image height of the ROI acquisition</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A description of the region of interest (ROI) captured in the image.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Multiple images (1-n) are acquired from regions of interest (ROI1, ROI2, ROI3, etc) on a slide. The roi_id is a number from 1-n representing the ROI captured on a slide.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The acquisition_id refers to the directory containing the ROI images for a slide. Together, the acquisition_id and the roi_id indicate the slide-ROI represented in the image.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Area normalized ion dose unit</t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,59 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Image width value of the ROI acquisition</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Units of image width of the ROI acquisition</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Image height value of the ROI acquisition</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Units of image height of the ROI acquisition</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -427,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -440,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -492,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -505,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -518,7 +557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -531,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -544,7 +583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -557,7 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AR1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -570,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
+    <comment ref="AS1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -583,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
+    <comment ref="AT1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -596,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0">
+    <comment ref="AU1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0">
+    <comment ref="AV1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -622,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0">
+    <comment ref="AW1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -635,7 +674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0">
+    <comment ref="AX1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -653,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>version</t>
   </si>
@@ -736,6 +775,27 @@
     <t>resolution_y_unit</t>
   </si>
   <si>
+    <t>max_x_width_value</t>
+  </si>
+  <si>
+    <t>max_x_width_unit</t>
+  </si>
+  <si>
+    <t>max_y_height_value</t>
+  </si>
+  <si>
+    <t>max_y_height_unit</t>
+  </si>
+  <si>
+    <t>roi_description</t>
+  </si>
+  <si>
+    <t>roi_id</t>
+  </si>
+  <si>
+    <t>acquisition_id</t>
+  </si>
+  <si>
     <t>area_normalized_ion_dose_unit</t>
   </si>
   <si>
@@ -754,18 +814,6 @@
     <t>end_datetime</t>
   </si>
   <si>
-    <t>max_x_width_value</t>
-  </si>
-  <si>
-    <t>max_x_width_unit</t>
-  </si>
-  <si>
-    <t>max_y_height_value</t>
-  </si>
-  <si>
-    <t>max_y_height_unit</t>
-  </si>
-  <si>
     <t>pixel_dwell_time_value</t>
   </si>
   <si>
@@ -818,6 +866,9 @@
   </si>
   <si>
     <t>nA</t>
+  </si>
+  <si>
+    <t>pA</t>
   </si>
   <si>
     <t>reagent_prep_protocols_io_doi</t>
@@ -1205,7 +1256,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU1"/>
+  <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1214,7 +1265,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:50">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,25 +1330,25 @@
         <v>27</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>36</v>
@@ -1309,13 +1360,13 @@
         <v>38</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>43</v>
@@ -1324,41 +1375,50 @@
         <v>44</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="AR1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>67</v>
+      <c r="AV1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="32">
+  <dataValidations count="33">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1396,76 +1456,80 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mm / um / nm." sqref="T2:T1048576">
       <formula1>'resolution_y_unit list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nA*hr/mm2." sqref="U2:U1048576">
-      <formula1>'area_normalize...dose_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="V2:V1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="U2:U1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="V2:V1048576">
+      <formula1>'max_x_width_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="W2:W1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="X2:X1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="X2:X1048576">
+      <formula1>'max_y_height_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Z2:Z1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AA2:AA1048576">
-      <formula1>'max_x_width_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AB2:AB1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nA*hr/mm2." sqref="AB2:AB1048576">
+      <formula1>'area_normalize...dose_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AC2:AC1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AC2:AC1048576">
-      <formula1>'max_y_height_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AD2:AD1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ms." sqref="AE2:AE1048576">
-      <formula1>'pixel_dwell_time_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AF2:AF1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AE2:AE1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm." sqref="AG2:AG1048576">
-      <formula1>'pixel_size_x_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AH2:AH1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AG2:AG1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm." sqref="AI2:AI1048576">
-      <formula1>'pixel_size_y_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Custom / Ionpath." sqref="AJ2:AJ1048576">
-      <formula1>'preparation_in...nt_vendor list'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Custom / MIBIscope 1 / MIBIscope 2." sqref="AK2:AK1048576">
-      <formula1>'preparation_in...ent_model list'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Xe." sqref="AL2:AL1048576">
-      <formula1>'primary_ion list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AM2:AM1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ms." sqref="AH2:AH1048576">
+      <formula1>'pixel_dwell_time_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nA." sqref="AN2:AN1048576">
-      <formula1>'primary_ion_current_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: float / integer / string." sqref="AQ2:AQ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm." sqref="AJ2:AJ1048576">
+      <formula1>'pixel_size_x_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AK2:AK1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm." sqref="AL2:AL1048576">
+      <formula1>'pixel_size_y_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Custom / Ionpath." sqref="AM2:AM1048576">
+      <formula1>'preparation_in...nt_vendor list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Custom / MIBIscope 1 / MIBIscope 2." sqref="AN2:AN1048576">
+      <formula1>'preparation_in...ent_model list'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Xe." sqref="AO2:AO1048576">
+      <formula1>'primary_ion list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AP2:AP1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nA / pA." sqref="AQ2:AQ1048576">
+      <formula1>'primary_ion_current_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: float / integer / string." sqref="AT2:AT1048576">
       <formula1>'segment_data_format list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: dual count / pulse count / intensity value." sqref="AR2:AR1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: dual count / pulse count / intensity value." sqref="AU2:AU1048576">
       <formula1>'signal_type list'!$A$1:$A$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -1484,7 +1548,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1566,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1556,12 +1620,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1579,17 +1643,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1607,7 +1671,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1681,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1625,7 +1689,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1643,17 +1712,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1671,17 +1740,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1827,7 +1896,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MIBI enum to replace Multiplexed Ion Beam Imaging
</commit_message>
<xml_diff>
--- a/docs/mibi/mibi-metadata.xlsx
+++ b/docs/mibi/mibi-metadata.xlsx
@@ -775,7 +775,7 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>Multiplex Ion Beam Imaging</t>
+    <t>MIBI</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -1482,7 +1482,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Multiplex Ion Beam Imaging." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: MIBI." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: protein." sqref="M2:M1048576">

</xml_diff>

<commit_message>
Updated MIBI enum to replace Multiplexed Ion Beam Imaging (#1166)
</commit_message>
<xml_diff>
--- a/docs/mibi/mibi-metadata.xlsx
+++ b/docs/mibi/mibi-metadata.xlsx
@@ -775,7 +775,7 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>Multiplex Ion Beam Imaging</t>
+    <t>MIBI</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -1482,7 +1482,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Multiplex Ion Beam Imaging." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: MIBI." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: protein." sqref="M2:M1048576">

</xml_diff>